<commit_message>
finished manual testing of v1
</commit_message>
<xml_diff>
--- a/documentation/Testing/TestingReport - Manual_v1.xlsx
+++ b/documentation/Testing/TestingReport - Manual_v1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
   <si>
     <t>Result</t>
   </si>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29:O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1879,10 +1879,12 @@
       <c r="N21" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="3"/>
+      <c r="O21" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="P21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -1922,10 +1924,12 @@
       <c r="N22" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="O22" s="3"/>
+      <c r="O22" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="P22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -1965,10 +1969,12 @@
       <c r="N23" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="O23" s="3"/>
+      <c r="O23" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="P23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
@@ -2235,10 +2241,12 @@
       <c r="N29" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="O29" s="3"/>
+      <c r="O29" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="P29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -2278,10 +2286,12 @@
       <c r="N30" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="O30" s="3"/>
+      <c r="O30" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="P30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2321,10 +2331,12 @@
       <c r="N31" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="O31" s="3"/>
+      <c r="O31" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="P31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">

</xml_diff>